<commit_message>
Refactor RSVP API to use Netlify Blobs for guest data storage and add export functionality for confirmations
</commit_message>
<xml_diff>
--- a/data/confirmaciones_boda.xlsx
+++ b/data/confirmaciones_boda.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -470,9 +470,29 @@
         <v>21/9/2025, 18:34:47</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>RAFAEL</v>
+      </c>
+      <c r="B4" t="str">
+        <v>PULIDO LOPEZ</v>
+      </c>
+      <c r="C4" t="str">
+        <v>NO</v>
+      </c>
+      <c r="D4" t="str">
+        <v/>
+      </c>
+      <c r="E4" t="str">
+        <v/>
+      </c>
+      <c r="F4" t="str">
+        <v>21/9/2025, 19:13:29</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor RSVP form and API to enhance guest data handling and allow multiple submissions
</commit_message>
<xml_diff>
--- a/data/confirmaciones_boda.xlsx
+++ b/data/confirmaciones_boda.xlsx
@@ -1,41 +1,50 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Projects\wedding-invitation\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29106CC-4E39-4DC5-92A6-2F463DF040ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Confirmaciones" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>NOMBRE</t>
+  </si>
+  <si>
+    <t>APELLIDOS</t>
+  </si>
+  <si>
+    <t>ACOMPAÑANTE</t>
+  </si>
+  <si>
+    <t>NOMBRE_ACOMPAÑANTE</t>
+  </si>
+  <si>
+    <t>APELLIDOS_ACOMPAÑANTE</t>
+  </si>
+  <si>
+    <t>FECHA_CONFIRMACION</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -65,13 +74,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,103 +413,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="2" max="2" width="25.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" customWidth="1"/>
-    <col min="5" max="5" width="25.83203125" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="20.875" customWidth="1"/>
+    <col min="2" max="2" width="25.875" customWidth="1"/>
+    <col min="3" max="3" width="15.875" customWidth="1"/>
+    <col min="4" max="4" width="20.875" customWidth="1"/>
+    <col min="5" max="5" width="25.875" customWidth="1"/>
+    <col min="6" max="6" width="20.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>NOMBRE</v>
-      </c>
-      <c r="B1" t="str">
-        <v>APELLIDOS</v>
-      </c>
-      <c r="C1" t="str">
-        <v>ACOMPAÑANTE</v>
-      </c>
-      <c r="D1" t="str">
-        <v>NOMBRE_ACOMPAÑANTE</v>
-      </c>
-      <c r="E1" t="str">
-        <v>APELLIDOS_ACOMPAÑANTE</v>
-      </c>
-      <c r="F1" t="str">
-        <v>FECHA_CONFIRMACION</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>JUAN</v>
-      </c>
-      <c r="B2" t="str">
-        <v>PEREZ</v>
-      </c>
-      <c r="C2" t="str">
-        <v>SÍ</v>
-      </c>
-      <c r="D2" t="str">
-        <v>MARIA</v>
-      </c>
-      <c r="E2" t="str">
-        <v>GARCIA</v>
-      </c>
-      <c r="F2" t="str">
-        <v>21/9/2025, 18:32:39</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>RAFAEL</v>
-      </c>
-      <c r="B3" t="str">
-        <v>PULIDO CIFUENTES</v>
-      </c>
-      <c r="C3" t="str">
-        <v>NO</v>
-      </c>
-      <c r="D3" t="str">
-        <v/>
-      </c>
-      <c r="E3" t="str">
-        <v/>
-      </c>
-      <c r="F3" t="str">
-        <v>21/9/2025, 18:34:47</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>RAFAEL</v>
-      </c>
-      <c r="B4" t="str">
-        <v>PULIDO LOPEZ</v>
-      </c>
-      <c r="C4" t="str">
-        <v>NO</v>
-      </c>
-      <c r="D4" t="str">
-        <v/>
-      </c>
-      <c r="E4" t="str">
-        <v/>
-      </c>
-      <c r="F4" t="str">
-        <v>21/9/2025, 19:13:29</v>
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
+    <ignoredError sqref="A1:F1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>